<commit_message>
sheet name: Overview → Schema Overview
</commit_message>
<xml_diff>
--- a/PocoPanda/Template/Template_Overview.xlsx
+++ b/PocoPanda/Template/Template_Overview.xlsx
@@ -1,22 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26731"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27628"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GitHubRepos\DapperPocoLab\Template\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GitHubRepos\PocoPanda\PocoPanda\Template\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{58632ADB-FADA-43F8-9D29-F2B623ED60AA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A6F11756-87E3-4836-9068-1377BA9C8BD1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-16320" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3315" yWindow="-14985" windowWidth="24495" windowHeight="13875" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Overview" sheetId="2" r:id="rId1"/>
+    <sheet name="Schema Overview" sheetId="2" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="ItemList">Overview!$A$6:$D$7</definedName>
+    <definedName name="ItemList">'Schema Overview'!$A$6:$D$7</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -360,9 +360,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 佈景主題">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 主題">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -400,7 +400,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -506,7 +506,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -648,7 +648,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>

</xml_diff>